<commit_message>
add corrections to 2022 Grav data
</commit_message>
<xml_diff>
--- a/Gravity/2022_Gravity.xlsx
+++ b/Gravity/2022_Gravity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kam98\Documents\Field Session\Gravity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kam98\Documents\Field Session\GitHub\fieldcamp_flinstones\Gravity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFCC43E-A13A-4464-8C98-0A4671DF5823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80ADF625-8A8B-4E10-BAD1-FC6F10429106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12877" yWindow="0" windowWidth="13125" windowHeight="15563" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12578" yWindow="0" windowWidth="13424" windowHeight="15563" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GROUP5 CG5-1" sheetId="1" r:id="rId1"/>
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -740,7 +740,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1058,7 +1058,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>